<commit_message>
proyecto gestor de actuaciones: Ajusto los css de la muestra de actividades pendientes de coordinar
</commit_message>
<xml_diff>
--- a/proyectos/gestorDeActuaciones/src/pruebasExcel/olin-3Incidencias.xlsx
+++ b/proyectos/gestorDeActuaciones/src/pruebasExcel/olin-3Incidencias.xlsx
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t xml:space="preserve">Código Cliente</t>
   </si>
@@ -199,10 +199,28 @@
     <t xml:space="preserve">olinct010</t>
   </si>
   <si>
+    <t xml:space="preserve">Málaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/ Málaga, 45, 5ºB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Manolo el del tambor</t>
   </si>
   <si>
+    <t xml:space="preserve">Fuengirola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/ Fuengirola, Urbanización el coto. 46</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fernando Fernandez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mijas costa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urbanización el Candado, calle Fuensanta, 45</t>
   </si>
 </sst>
 </file>
@@ -212,7 +230,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -233,12 +251,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -309,7 +321,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -392,11 +404,11 @@
   </sheetPr>
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S4" activeCellId="0" sqref="S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.33"/>
@@ -516,6 +528,12 @@
       <c r="I2" s="0" t="n">
         <v>266000</v>
       </c>
+      <c r="Q2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -525,7 +543,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>222222222</v>
@@ -544,6 +562,12 @@
       </c>
       <c r="I3" s="0" t="n">
         <v>266001</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,7 +578,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>333333333</v>
@@ -573,6 +597,12 @@
       </c>
       <c r="I4" s="0" t="n">
         <v>266002</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>